<commit_message>
Werk van les KBSa 20/11/2023
Analyse t/m user case beschrijving + tijdschrijven van iedereen die in de les was
</commit_message>
<xml_diff>
--- a/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
+++ b/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\docs\oplevering\08Projectdocumentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEA7DDE-E69C-4133-96A9-7DDA6339D8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB39B9E-0137-4A36-B2E5-B097EF59E1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1290" windowWidth="14790" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marvin" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="30">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -585,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -653,7 +653,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -757,6 +757,20 @@
         <v>120</v>
       </c>
       <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45250</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1179,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1249,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>16.666666666666668</v>
+        <v>18.666666666666668</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1247,7 +1261,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>151.33333333333334</v>
+        <v>149.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1352,6 +1366,20 @@
       </c>
       <c r="D15" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45250</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1377,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,7 +1461,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>21.5</v>
+        <v>23.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1445,7 +1473,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>146.5</v>
+        <v>144.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1583,6 +1611,20 @@
       </c>
       <c r="C18">
         <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45250</v>
+      </c>
+      <c r="C19">
+        <v>120</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1608,25 +1650,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1852,33 +1875,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1896,4 +1912,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update tijdschrijven w les 23/11 inc.
</commit_message>
<xml_diff>
--- a/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
+++ b/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\docs\oplevering\08Projectdocumentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB39B9E-0137-4A36-B2E5-B097EF59E1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B0EA00-CD76-4792-B1F7-4FEAD8FA0AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1290" windowWidth="14790" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1290" windowWidth="14790" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marvin" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="30">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -585,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="D18" sqref="A17:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -653,7 +653,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -771,6 +771,34 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45252</v>
+      </c>
+      <c r="C17">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45253</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -797,10 +825,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A15" sqref="A15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +881,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -865,7 +893,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -955,6 +983,34 @@
         <v>120</v>
       </c>
       <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45252</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45253</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -981,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A17" sqref="A17:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1093,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1049,7 +1105,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1168,6 +1224,34 @@
       </c>
       <c r="D16" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45252</v>
+      </c>
+      <c r="C17">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45253</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1193,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1333,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>18.666666666666668</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1261,7 +1345,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>149.33333333333334</v>
+        <v>147.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1379,6 +1463,20 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45253</v>
+      </c>
+      <c r="C17">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1407,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
@@ -1650,6 +1748,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1875,26 +1992,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1912,30 +2036,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tijdschrijven vandaag + gister lessen want niemand doet t self :clown:
</commit_message>
<xml_diff>
--- a/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
+++ b/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chmen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\docs\oplevering\08Projectdocumentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEBDB7B-CA90-4995-92AF-EB08FC0D79A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAC7F2F-1D6C-41BF-964B-7FA933D2644D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marvin" sheetId="7" r:id="rId1"/>
@@ -28,6 +28,17 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="47">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -167,7 +178,16 @@
     <t>Thuis alleen gewerkt</t>
   </si>
   <si>
-    <t>27/11/20203</t>
+    <t>Datum word verkeerd geprint. Staat wel correct in edit balk boven in excel</t>
+  </si>
+  <si>
+    <t>zoinks scoob</t>
+  </si>
+  <si>
+    <t>KBS momentje geplanned</t>
+  </si>
+  <si>
+    <t>Lonely aanwezig in teams D:</t>
   </si>
 </sst>
 </file>
@@ -249,9 +269,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -618,22 +638,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A24" sqref="A24:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -641,7 +661,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -649,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -657,7 +677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -665,37 +685,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>32.5</v>
+        <v>36.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>135.5</v>
+        <v>131.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -709,7 +729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -723,7 +743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -737,7 +757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -751,7 +771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -765,7 +785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -779,7 +799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -793,7 +813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -807,7 +827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -821,7 +841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -835,7 +855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -849,7 +869,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -863,7 +883,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -874,7 +894,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -888,7 +908,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -897,6 +917,37 @@
       </c>
       <c r="C23">
         <v>150</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C24">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C25">
+        <v>120</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -922,22 +973,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScale="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView view="pageLayout" zoomScale="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -945,7 +996,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -953,7 +1004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -961,7 +1012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -969,37 +1020,40 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1013,7 +1067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1027,7 +1081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1041,7 +1095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1055,7 +1109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1069,7 +1123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1151,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1111,7 +1165,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1125,18 +1179,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
-        <v>43</v>
+      <c r="B18" s="2">
+        <v>45257</v>
       </c>
       <c r="C18">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1150,7 +1204,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1161,7 +1215,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1175,7 +1229,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1184,6 +1238,34 @@
       </c>
       <c r="C22">
         <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C23">
+        <v>120</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C24">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1209,22 +1291,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="D21" sqref="A21:D21"/>
+      <selection activeCell="A22" sqref="A22:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +1314,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1248,7 +1330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1256,37 +1338,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1300,7 +1382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1314,7 +1396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1410,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1342,7 +1424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1356,7 +1438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1370,7 +1452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1384,7 +1466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1398,7 +1480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1412,7 +1494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1426,7 +1508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1440,7 +1522,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1451,7 +1533,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1463,6 +1545,34 @@
       </c>
       <c r="D21" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C22">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C23">
+        <v>120</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1488,22 +1598,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="C24" sqref="A24:C24"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1621,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1519,7 +1629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1535,37 +1645,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>36.833333333333336</v>
+        <v>42.833333333333336</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>131.16666666666666</v>
+        <v>125.16666666666666</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1579,7 +1689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1593,7 +1703,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1607,7 +1717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1621,7 +1731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1635,7 +1745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1649,7 +1759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1663,7 +1773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1677,7 +1787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1691,7 +1801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1705,7 +1815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1719,7 +1829,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1730,7 +1840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1741,7 +1851,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1752,7 +1862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1766,7 +1876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1778,6 +1888,48 @@
       </c>
       <c r="D24" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C25">
+        <v>120</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C26">
+        <v>120</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45266</v>
+      </c>
+      <c r="C27">
+        <v>120</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1803,22 +1955,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A21" sqref="A21:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1978,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1834,7 +1986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1842,7 +1994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1850,37 +2002,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>25.5</v>
+        <v>29.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>142.5</v>
+        <v>138.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1894,7 +2046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1908,7 +2060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1922,7 +2074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1936,7 +2088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1950,7 +2102,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1961,7 +2113,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1975,7 +2127,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1986,7 +2138,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2000,7 +2152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2011,7 +2163,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2025,7 +2177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2034,6 +2186,34 @@
       </c>
       <c r="C20">
         <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C21">
+        <v>120</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C22">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2059,13 +2239,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2295,28 +2474,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2342,9 +2512,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Brr kleine aanpassing FO, Voorgang rapp w50 gemaakt
</commit_message>
<xml_diff>
--- a/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
+++ b/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdy_gadgets\docs\oplevering\08Projectdocumentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\docs\oplevering\08Projectdocumentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61E1335-6B00-4B69-80E2-90CDAE989460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD14F87-97BD-43CE-B92D-7B92E858A43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="14790" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marvin" sheetId="7" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="51">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>Lonely aanwezig in teams D:</t>
+  </si>
+  <si>
+    <t>Les + doorgewerkt</t>
+  </si>
+  <si>
+    <t>Werken in de trein brrr</t>
+  </si>
+  <si>
+    <t>Eigen conversie maatregel</t>
+  </si>
+  <si>
+    <t>Eigen conversie maatregel + voortgang rapport</t>
   </si>
 </sst>
 </file>
@@ -269,9 +281,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -638,22 +650,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -661,7 +673,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -669,7 +681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -677,7 +689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -685,37 +697,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -729,7 +741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -743,7 +755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -757,7 +769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -771,7 +783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -785,7 +797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -799,7 +811,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -813,7 +825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -827,7 +839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -841,7 +853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -855,7 +867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -869,7 +881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -883,7 +895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -894,7 +906,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -908,7 +920,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -922,7 +934,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -936,7 +948,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -950,7 +962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -964,7 +976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -978,7 +990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -989,6 +1001,20 @@
         <v>120</v>
       </c>
       <c r="D28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C29">
+        <v>120</v>
+      </c>
+      <c r="D29" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1015,22 +1041,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A12" zoomScale="83" zoomScalePageLayoutView="83" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1064,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1054,7 +1080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1062,40 +1088,40 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>38.5</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>129.5</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1109,7 +1135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1123,7 +1149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1137,7 +1163,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1151,7 +1177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1165,7 +1191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1179,7 +1205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1193,7 +1219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1207,7 +1233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1221,7 +1247,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1232,7 +1258,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1246,7 +1272,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1257,7 +1283,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1271,7 +1297,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1282,7 +1308,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1296,7 +1322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1310,7 +1336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1324,7 +1350,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1332,13 +1358,13 @@
         <v>45271</v>
       </c>
       <c r="C26">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1349,6 +1375,20 @@
         <v>120</v>
       </c>
       <c r="D27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C28">
+        <v>120</v>
+      </c>
+      <c r="D28" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1375,22 +1415,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1398,7 +1438,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1406,7 +1446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1414,7 +1454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1422,10 +1462,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1437,7 +1477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1449,10 +1489,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1466,7 +1506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1494,7 +1534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1508,7 +1548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1522,7 +1562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1550,7 +1590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1564,7 +1604,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1578,7 +1618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1592,7 +1632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1606,7 +1646,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1617,7 +1657,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1631,7 +1671,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1645,7 +1685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1659,7 +1699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1670,7 +1710,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1684,7 +1724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1698,7 +1738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1711,6 +1751,9 @@
       <c r="D27" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1735,22 +1778,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1758,7 +1801,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1766,7 +1809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1774,7 +1817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1782,37 +1825,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>47.333333333333336</v>
+        <v>51.583333333333336</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>120.66666666666666</v>
+        <v>116.41666666666666</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1826,7 +1869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1840,7 +1883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1854,7 +1897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1868,7 +1911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1882,7 +1925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1896,7 +1939,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1910,7 +1953,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1924,7 +1967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1938,7 +1981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1952,7 +1995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1966,7 +2009,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1977,7 +2020,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1988,7 +2031,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1999,7 +2042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2013,7 +2056,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2027,7 +2070,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2041,7 +2084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2055,7 +2098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -2069,7 +2112,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -2080,10 +2123,10 @@
         <v>150</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2095,6 +2138,48 @@
       </c>
       <c r="D29" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C30">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C31">
+        <v>120</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C32">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2120,22 +2205,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="21.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.73046875" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2143,7 +2228,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2151,7 +2236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2159,7 +2244,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2167,37 +2252,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>29.5</v>
+        <v>31.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>138.5</v>
+        <v>136.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2211,7 +2296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2225,7 +2310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2239,7 +2324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2253,7 +2338,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2267,7 +2352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2278,7 +2363,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2292,7 +2377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2303,7 +2388,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2317,7 +2402,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2328,7 +2413,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2342,7 +2427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2353,7 +2438,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2367,7 +2452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2378,6 +2463,20 @@
         <v>120</v>
       </c>
       <c r="D22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C23">
+        <v>120</v>
+      </c>
+      <c r="D23" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
owo ewe awa iwi lijkt op kiwi
</commit_message>
<xml_diff>
--- a/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
+++ b/docs/oplevering/08Projectdocumentatie/Tijdschrijfformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chmen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\docs\oplevering\08Projectdocumentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED870C3E-8D0A-4D10-9353-2172EBF448E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99D6878-BE95-4F0E-8513-6A4443A6FBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="480" windowWidth="14790" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marvin" sheetId="7" r:id="rId1"/>
@@ -27,11 +27,24 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Marvin!$A$1:$D$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="59">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -199,6 +212,15 @@
   </si>
   <si>
     <t>Conversie maatregel realiseren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KBS a les </t>
+  </si>
+  <si>
+    <t>Gewerkt in trein brr</t>
+  </si>
+  <si>
+    <t>Trein go brr</t>
   </si>
 </sst>
 </file>
@@ -280,9 +302,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -655,16 +677,16 @@
       <selection activeCell="A30" sqref="A30:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -672,7 +694,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -680,7 +702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -688,7 +710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -696,10 +718,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -711,7 +733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -723,10 +745,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -740,7 +762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -754,7 +776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -768,7 +790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -782,7 +804,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -796,7 +818,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -810,7 +832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -824,7 +846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -838,7 +860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -852,7 +874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -866,7 +888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -880,7 +902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -894,7 +916,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -905,7 +927,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -919,7 +941,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -933,7 +955,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -947,7 +969,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -961,7 +983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -975,7 +997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -989,7 +1011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1017,7 +1039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1055,16 +1077,16 @@
       <selection activeCell="A32" sqref="A32:D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1094,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1080,7 +1102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1096,10 +1118,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1111,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1123,13 +1145,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1143,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1157,7 +1179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1171,7 +1193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1185,7 +1207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1199,7 +1221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1227,7 +1249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1241,7 +1263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1255,7 +1277,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1266,7 +1288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1280,7 +1302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1291,7 +1313,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1305,7 +1327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1316,7 +1338,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1330,7 +1352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1344,7 +1366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1358,7 +1380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1372,7 +1394,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1386,7 +1408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1400,7 +1422,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1411,7 +1433,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1422,7 +1444,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1433,7 +1455,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1471,16 +1493,16 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1488,7 +1510,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1496,7 +1518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1504,7 +1526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1512,10 +1534,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1527,7 +1549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1539,10 +1561,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1556,7 +1578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1570,7 +1592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1584,7 +1606,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1598,7 +1620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1612,7 +1634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1626,7 +1648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1640,7 +1662,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1654,7 +1676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1668,7 +1690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1682,7 +1704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1696,7 +1718,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1707,7 +1729,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1721,7 +1743,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1735,7 +1757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1749,7 +1771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1760,7 +1782,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1774,7 +1796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1788,7 +1810,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1825,22 +1847,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:D30"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1848,7 +1870,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1856,7 +1878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1864,7 +1886,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1872,37 +1894,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>49.333333333333336</v>
+        <v>52.583333333333336</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>118.66666666666666</v>
+        <v>115.41666666666666</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1916,7 +1938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1930,7 +1952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1944,7 +1966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1958,7 +1980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1972,7 +1994,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1986,7 +2008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2000,7 +2022,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2014,7 +2036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2028,7 +2050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2042,7 +2064,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2056,7 +2078,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2067,7 +2089,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2078,7 +2100,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2089,7 +2111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2103,7 +2125,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2117,7 +2139,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2131,7 +2153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2145,7 +2167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -2159,7 +2181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -2173,7 +2195,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2187,17 +2209,59 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B30" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="2">
+        <v>45274</v>
+      </c>
+      <c r="C31">
+        <v>120</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="2">
         <v>45279</v>
       </c>
-      <c r="C30">
-        <v>120</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C32">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="2">
+        <v>45279</v>
+      </c>
+      <c r="C33">
+        <v>120</v>
+      </c>
+      <c r="D33" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2224,22 +2288,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:D40"/>
+    <sheetView view="pageLayout" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2247,7 +2311,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2255,7 +2319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2263,7 +2327,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2271,10 +2335,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2286,7 +2350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2298,10 +2362,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2315,7 +2379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2329,7 +2393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2343,7 +2407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2357,7 +2421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2371,7 +2435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2382,7 +2446,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2396,7 +2460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2407,7 +2471,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2421,7 +2485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2432,7 +2496,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2446,7 +2510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2457,7 +2521,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -2468,7 +2532,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2482,7 +2546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2496,7 +2560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2510,7 +2574,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2524,7 +2588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2538,7 +2602,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2552,7 +2616,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2566,7 +2630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -2580,7 +2644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -2594,7 +2658,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2608,7 +2672,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -2622,7 +2686,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2636,23 +2700,26 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2">
         <v>45279</v>
       </c>
+      <c r="C34">
+        <v>120</v>
+      </c>
       <c r="D34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>45279</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -2663,17 +2730,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>45280</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>45281</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2681,20 +2748,6 @@
         <v>45282</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="2">
-        <v>45279</v>
-      </c>
-      <c r="C40">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2716,6 +2769,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2941,41 +3013,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2999,9 +3040,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>